<commit_message>
[testing] updated test cases
</commit_message>
<xml_diff>
--- a/Test Files/Unit Tests.xlsx
+++ b/Test Files/Unit Tests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
   <si>
     <t xml:space="preserve">S/N</t>
   </si>
@@ -155,16 +155,142 @@
     <t xml:space="preserve">KeyValue.TryParse()</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test1.cfg, Test1.seq, Test1.czl
-Data: Appendix A, Appendix B, Appendix C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test2.cfg, Test2.seq, Test2.czl
-Data: Appendix D, Appendix E, Appendix F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test3.cfg, Test3.seq, Test3.czl
-Data: Appendix G, Appendix H, Appendix I</t>
+    <t xml:space="preserve">File: Test1.cfg
+Data:
+INTERSECTING-POINTS
+    A=1
+    B=2
+    C=2
+    D=2
+    E=1
+    F=2
+    G=2
+    H=2
+    I=1
+    J=4
+    K=4
+    L=4
+    M=4
+    N=4
+    O=1
+    P=8
+    Q=8
+    R=8
+    S=8
+    T=8
+    U=1
+    V=16
+    W=16
+    X=32
+    Y=32
+    Z=64
+END-INTERSECTING-POINTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File will parse correctly, all data is valid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File: Test2.cfg
+Data:
+INTERSECTING-POINTS
+  A=1
+  B=2
+  C=2
+  D=2
+  E=1
+  F=2
+  G=2
+  H=2
+  I=1
+  J=4
+  K=4
+  L=4
+  M=4
+  N=4
+  O=1
+  P=8
+  Q=8
+  R=8
+  S=8
+  T=8
+  U=1
+  V=16
+  W=16
+  X=32
+  Y=32
+  Z=64
+  z=64
+END-INTERSECTING-POINTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File will parse correctly, contains invalid data with lowercase keyvalue that doesn’t match regular expression.
+KeyValue.TryParse() will return error for this KeyValue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File: Test3.cfg
+Data:
+INTERSECTING-POINTS
+  AAA=1
+  B=
+  C,2
+  D=XXXX
+  E=1
+  F=2
+  G=2
+  H=2
+  I=1
+  J=4
+  K=4
+  L=4
+  M=4
+  N=4
+  O=1
+  P=8
+  Q=8
+  R=8
+  S=8
+  T=8
+  U=1
+  V=16
+  W=16
+  X=32
+  Y=32
+  Z=64
+END-INTERSECTING-POINTS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Contains invalid and illegal data.
+KeyValue.TryParse() will return error invalid data for lines without “</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">” symbol.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Crozzle.Score()</t>
@@ -762,18 +888,30 @@
     <t xml:space="preserve">Crozzle.Validate()</t>
   </si>
   <si>
+    <t xml:space="preserve">File: Test1.cfg, Test1.seq, Test1.czl
+Data: Appendix A, Appendix B, Appendix C</t>
+  </si>
+  <si>
     <t xml:space="preserve">Files will parse correctly.
 Files will validate successfully.
 Parse success will be logged.
 Crozzle will display correctly with all words in word list and correct score displayed.</t>
   </si>
   <si>
+    <t xml:space="preserve">File: Test2.cfg, Test2.seq, Test2.czl
+Data: Appendix D, Appendix E, Appendix F</t>
+  </si>
+  <si>
     <t xml:space="preserve">Files will parse correctly.
 Files will not validate successfully. Crozzle is not valid with Test2.cfg. Errors will be logged for each invalid section of data.
 Parse success will be logged.
 Crozzle will display with vlid data displayed and the invalid Crozzle score displayed.</t>
   </si>
   <si>
+    <t xml:space="preserve">File: Test3.cfg, Test3.seq, Test3.czl
+Data: Appendix G, Appendix H, Appendix I</t>
+  </si>
+  <si>
     <t xml:space="preserve">Files will fail to parse due to invalid data.
 Files will not validate successfully. Crozzle is not valid due to invalid data, illegal data, missing data, Test3.cfg invalid. Errors will be logged for every section of invalid and illegal data encountered.
 Crozzle will display with as much valid data as can be found.
@@ -783,6 +921,33 @@
     <t xml:space="preserve">Crozzle.ToStringHTML()</t>
   </si>
   <si>
+    <t xml:space="preserve">File: Test1.cfg, Test1.czl
+Data: Appendix A, Appendix C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File will parse correctly, all data is valid.
+Crozzle.ToStringHTML() will create legal HTML.
+Crozle will display in the given style.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File: Test2.cfg, Test2.czl
+Data: Appendix D, Appendix F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File will parse correctly, invalid data including duplicate will not be processed. 
+Valid data will be output to HTML string by Crozzle.ToStringHTML() and invalid data will be displayed in error log.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File: Test3.cfg, Test3.czl
+Data: Appendix G, Appendix I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File is invalid and cannot be parsed. 
+Error parsing file will be logged.
+Any valid data will be processed into HTML and returned by Crozzle.ToStringHTML().
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">CrozzleMap.GroupCount()</t>
   </si>
   <si>
@@ -803,9 +968,6 @@
   <si>
     <t xml:space="preserve">File: Test1.cfg
 Data: Appendix A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File will parse correctly, all data is valid.</t>
   </si>
   <si>
     <t xml:space="preserve">File: Test2.cfg
@@ -995,7 +1157,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1015,14 +1177,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
@@ -1067,9 +1221,9 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1267,7 +1421,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="406.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="str">
         <f aca="false">TEXT(ROW(A10)-1,"00")</f>
         <v>09</v>
@@ -1281,11 +1435,13 @@
       <c r="D10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="420" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="str">
         <f aca="false">TEXT(ROW(A11)-1,"00")</f>
         <v>10</v>
@@ -1297,13 +1453,15 @@
         <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="406.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="str">
         <f aca="false">TEXT(ROW(A12)-1,"00")</f>
         <v>11</v>
@@ -1315,9 +1473,11 @@
         <v>26</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
@@ -1330,13 +1490,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -1350,13 +1510,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -1370,13 +1530,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1390,13 +1550,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -1410,13 +1570,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1430,13 +1590,13 @@
         <v>6</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1450,13 +1610,13 @@
         <v>7</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1470,13 +1630,13 @@
         <v>7</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -1490,54 +1650,58 @@
         <v>7</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="str">
+    <row r="22" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="str">
         <f aca="false">TEXT(ROW(A22)-1,"00")</f>
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="n">
+      <c r="B22" s="6" t="n">
         <v>8</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="str">
+    <row r="23" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="str">
         <f aca="false">TEXT(ROW(A23)-1,"00")</f>
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="n">
+      <c r="B23" s="6" t="n">
         <v>8</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="str">
         <f aca="false">TEXT(ROW(A24)-1,"00")</f>
         <v>23</v>
@@ -1546,12 +1710,14 @@
         <v>8</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
@@ -1564,10 +1730,10 @@
         <v>9</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1582,10 +1748,10 @@
         <v>9</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -1600,10 +1766,10 @@
         <v>9</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -1618,13 +1784,13 @@
         <v>10</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -1638,13 +1804,13 @@
         <v>10</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -1658,13 +1824,13 @@
         <v>10</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -1678,13 +1844,13 @@
         <v>11</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -1698,19 +1864,19 @@
         <v>11</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="str">
+      <c r="A33" s="5" t="str">
         <f aca="false">TEXT(ROW(A33)-1,"00")</f>
         <v>32</v>
       </c>
@@ -1718,73 +1884,73 @@
         <v>11</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="str">
+      <c r="A34" s="5" t="str">
         <f aca="false">TEXT(ROW(A34)-1,"00")</f>
         <v>33</v>
       </c>
-      <c r="B34" s="8" t="n">
+      <c r="B34" s="6" t="n">
         <v>12</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="str">
+      <c r="A35" s="5" t="str">
         <f aca="false">TEXT(ROW(A35)-1,"00")</f>
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="n">
+      <c r="B35" s="6" t="n">
         <v>12</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="str">
+      <c r="A36" s="5" t="str">
         <f aca="false">TEXT(ROW(A36)-1,"00")</f>
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="n">
+      <c r="B36" s="6" t="n">
         <v>12</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>

</xml_diff>

<commit_message>
[testing] added new test files in old file format for testing
</commit_message>
<xml_diff>
--- a/Test Files/Unit Tests.xlsx
+++ b/Test Files/Unit Tests.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arran\Projects\SIT323-Assignment-1\Test Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{764389C5-C26B-429A-B34C-7408F71D3FC2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,142 +25,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
-  <si>
-    <t xml:space="preserve">S/N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assessment Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actual Output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pass/Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validator.IsBoolean()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test1.cfg
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
+  <si>
+    <t>S/N</t>
+  </si>
+  <si>
+    <t>Assessment Item</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Input Data</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Output</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Validator.IsBoolean()</t>
+  </si>
+  <si>
+    <t>File: Test1.cfg
 Data:
 CROZZLE-OUTPUT
     UPPERCASE=true
 END-CROZZLE-OUTPUT</t>
   </si>
   <si>
-    <t xml:space="preserve">Test1.cfg will parse and validate this option correctly.
+    <t>Test1.cfg will parse and validate this option correctly.
 Validator.IsBoolean() will return true.
 Crozzle GUI will output with all valid sequences in uppercase formatting.</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test3.cfg
+    <t>File: Test3.cfg
 Data:
 CROZZLE-OUTPUT
     UPPERCASE=uppercase
 END-CROZZLE-OUTPUT</t>
   </si>
   <si>
-    <t xml:space="preserve">Test3.cfg will log an error when validating this option as there is no valid boolean option present.
-Validator.IsBoolean() will return false.
-Test3.cfg line 17 contains invalid data error message will be thrown.
-Crozzle GUI will output all valid sequences in uppercase as default.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validator.IsInt32()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test1.czl
+    <t>Validator.IsInt32()</t>
+  </si>
+  <si>
+    <t>File: Test1.czl
 Data:
 CROZZLE-SIZE
     SIZE=10,15
 END-CROZZLE-SIZE</t>
   </si>
   <si>
-    <t xml:space="preserve">Test1.czl will be parse and validate this option correctly.
+    <t>Test1.czl will be parse and validate this option correctly.
 Validator.IsInt32() will return true.
 Crozzle GUI will display a 10 row by 15 column Crozzle display.</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test2.czl
-Data:
-CROZZLE-SIZE
-    SIZE=-10,15
-END-CROZZLE-SIZE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test2.czl will parse as invalid due to the "-10" being an invalid size value, but Validator.IsInt32() will return true as the number is technically a valid Int32.
-Crozzle will log an error in parsing Test2.czl file CROZZLE-SIZE.
-Test2.czl line 10 error message will be thrown.
-Crozzle program will switch -10 to 10 and display a 10 row by 15 column GUI.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test3.czl
+    <t>File: Test3.czl
 Data:
 CROZZLE-SIZE
     SIZE=10,y
 END-CROZZLE-SIZE</t>
   </si>
   <si>
-    <t xml:space="preserve">Test3.czl will fail parsing and validation.
-Validator.IsInt32() will return false.
-A log message of failing to parse Test3.czl will be added.
-Test3.czl line 10 invalid data message will be thrown.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validator.IsHexColourCode()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test1.cfg
+    <t>Validator.IsHexColourCode()</t>
+  </si>
+  <si>
+    <t>File: Test1.cfg
 Data:
 CROZZLE-OUTPUT
     BGCOLOUR-EMPTY-TD=#777777
 END-CROZZLE-OUTPUT</t>
   </si>
   <si>
-    <t xml:space="preserve">Test1.cfg will parse and validate this option correctly.
+    <t>Test1.cfg will parse and validate this option correctly.
 Validator.IsHexColourCode() will return true.
 Crozzle GUI will output with all empty cells as hex colour code #777777 (grey).</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test2.cfg
+    <t>File: Test2.cfg
 Data:
 CROZZLE-OUTPUT
     BGCOLOUR-EMPTY-TD=#777
 END-CROZZLE-OUTPUT</t>
   </si>
   <si>
-    <t xml:space="preserve">Test2.cfg will parse and validate this option correctly.
+    <t>Test2.cfg will parse and validate this option correctly.
 Validator.IsHexColourCode() will return true, this is a valid hex colour code.
 Crozzle GUI will output with all empty cells as hex colour code #777 (grey).</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test3.cfg
+    <t>File: Test3.cfg
 Data:
 CROZZLE-OUTPUT
     BGCOLOUR-EMPTY-TD=777777
 END-CROZZLE-OUTPUT</t>
   </si>
   <si>
-    <t xml:space="preserve">Test3.cfg will log an error when validating this option as there is no valid hex colour code present.
-Validator.IsHexColourCode() will return false.
-Test3.cfg line 19 contains invalid data error message will be thrown.
-Crozzle GUI will output all valid sequences with empty TD element colour #777777 (grey) as default.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KeyValue.TryParse()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test1.cfg
+    <t>KeyValue.TryParse()</t>
+  </si>
+  <si>
+    <t>File: Test1.cfg
 Data:
 INTERSECTING-POINTS
     A=1
@@ -187,10 +161,10 @@
 END-INTERSECTING-POINTS</t>
   </si>
   <si>
-    <t xml:space="preserve">File will parse correctly, all data is valid.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test2.cfg
+    <t>File will parse correctly, all data is valid.</t>
+  </si>
+  <si>
+    <t>File: Test2.cfg
 Data:
 INTERSECTING-POINTS
   A=1
@@ -223,11 +197,11 @@
 END-INTERSECTING-POINTS</t>
   </si>
   <si>
-    <t xml:space="preserve">File will parse correctly, contains invalid data with lowercase keyvalue that doesn’t match regular expression.
+    <t>File will parse correctly, contains invalid data with lowercase keyvalue that doesn’t match regular expression.
 KeyValue.TryParse() will return error for this KeyValue.</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test3.cfg
+    <t>File: Test3.cfg
 Data:
 INTERSECTING-POINTS
   AAA=1
@@ -267,19 +241,19 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Contains invalid and illegal data.
+      <t>Contains invalid and illegal data.
 KeyValue.TryParse() will return error invalid data for lines without “</t>
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">=</t>
+      <t>=</t>
     </r>
     <r>
       <rPr>
@@ -289,14 +263,14 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">” symbol.</t>
+      <t>” symbol.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Crozzle.Score()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test1.cfg, Test1.seq, Test1.czl
+    <t>Crozzle.Score()</t>
+  </si>
+  <si>
+    <t>File: Test1.cfg, Test1.seq, Test1.czl
 Data (Test1.cfg):
 SEQUENCES-IN-CROZZLE
   MINIMUM-HORIZONTAL=1
@@ -421,12 +395,12 @@
 WENDY,10,5,391,406</t>
   </si>
   <si>
-    <t xml:space="preserve">All files will parse and validate correclty.
+    <t>All files will parse and validate correclty.
 Crozzle.Score() will return 192 for the score.
 Crozzle will display correctly in the GUI with the input sequences stated and display the score 192.</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test2.cfg, Test2.seq, Test2.czl
+    <t>File: Test2.cfg, Test2.seq, Test2.czl
 Data (Test2.cfg):
 SEQUENCES-IN-CROZZLE
   MINIMUM-HORIZONTAL=10
@@ -552,12 +526,12 @@
 WENDY,10,5,391,406</t>
   </si>
   <si>
-    <t xml:space="preserve">All files will parse correctly but the Crozzle is invalid as it exceeds the maximum vertical sequences permissible in the Test2.cfg file.
+    <t>All files will parse correctly but the Crozzle is invalid as it exceeds the maximum vertical sequences permissible in the Test2.cfg file.
 Crozzle.Score() will return 69 for the score.
 Crozzle will display correctly in the GUI with the input sequences stated but display the invalid Crozzle score text..</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test3.cfg, Test3.seq, Test3.czl
+    <t>File: Test3.cfg, Test3.seq, Test3.czl
 Data (Test3.cfg):
 SEQUENCES-IN-CROZZLE
   MINIMUM-HORIZONTAL=2
@@ -676,16 +650,16 @@
 WENDY,10,5,391,406</t>
   </si>
   <si>
-    <t xml:space="preserve">All files will fail parsing and validation.
+    <t>All files will fail parsing and validation.
 Crozzle.Score() will throw an invalid exception and not return a score.
 An invalid data error will be logged for all test files.
 An error message will be displayed for each error including Test3.cfg invalid intersecting points, Test3.cfg invalid sequence limit, minimum exceeds maximum, Test3.seq invalid data, Test3.czl invalid location.</t>
   </si>
   <si>
-    <t xml:space="preserve">CrozzleSequences.CheckDuplicateWords()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test1.czl, Test1.seq
+    <t>CrozzleSequences.CheckDuplicateWords()</t>
+  </si>
+  <si>
+    <t>File: Test1.czl, Test1.seq
 Data (Test1.czl):
 HORIZONTAL-SEQUENCES
     SEQUENCE=PETER,LOCATION=1,1
@@ -747,12 +721,12 @@
 WENDY,10,5,391,406</t>
   </si>
   <si>
-    <t xml:space="preserve">Test1.czl and Test1.seq will parse and validate correctly.
+    <t>Test1.czl and Test1.seq will parse and validate correctly.
 CrozzleSequences.CheckDuplicateWords() will return 0.
 Crozzle GUI will output Crozzle containing all the sequences from file correctly.</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test2.czl, Test2.seq
+    <t>File: Test2.czl, Test2.seq
 Data (Test2.czl):
 HORIZONTAL-SEQUENCES
     SEQUENCE=ROBERT,LOCATION=1,2
@@ -815,7 +789,7 @@
 WENDY,10,5,391,406</t>
   </si>
   <si>
-    <t xml:space="preserve">Files will parse correctly, file Test2.czl is invalid due to duplicate words exceeding duplicate word limit.
+    <t>Files will parse correctly, file Test2.czl is invalid due to duplicate words exceeding duplicate word limit.
 CrozzleSequences.CheckDuplicateWords() will return 4 duplicate words.
 Log error for invalid Crozzle due to excessive duplicate words.
 Display error message for duplicate words in Test2.czl word AL with 1 duplicate.
@@ -823,7 +797,7 @@
 Test2.czl word RON with 1 duplicate.</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test3.czl, Test3.seq
+    <t>File: Test3.czl, Test3.seq
 Data (Test3.czl):
 HORIZONTAL-SEQUENCES
     SEQUENCE=ROBERT,LOCATION=aaa,2
@@ -879,66 +853,66 @@
 WENDY,10,5,391,406</t>
   </si>
   <si>
-    <t xml:space="preserve">Files will fail to parse with incorrect data, file Test3.czl is invalid due to invalid and data missing.
+    <t>Files will fail to parse with incorrect data, file Test3.czl is invalid due to invalid and data missing.
 CrozzleSequences.CheckDuplicateWords() will return 1 duplicate word.
 Log error for invalid Crozzle due to excessive duplicate words.
 Display error message for duplicate words in Test3.czl word AL with 1 duplicate.</t>
   </si>
   <si>
-    <t xml:space="preserve">Crozzle.Validate()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test1.cfg, Test1.seq, Test1.czl
+    <t>Crozzle.Validate()</t>
+  </si>
+  <si>
+    <t>File: Test1.cfg, Test1.seq, Test1.czl
 Data: Appendix A, Appendix B, Appendix C</t>
   </si>
   <si>
-    <t xml:space="preserve">Files will parse correctly.
+    <t>Files will parse correctly.
 Files will validate successfully.
 Parse success will be logged.
 Crozzle will display correctly with all words in word list and correct score displayed.</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test2.cfg, Test2.seq, Test2.czl
+    <t>File: Test2.cfg, Test2.seq, Test2.czl
 Data: Appendix D, Appendix E, Appendix F</t>
   </si>
   <si>
-    <t xml:space="preserve">Files will parse correctly.
+    <t>Files will parse correctly.
 Files will not validate successfully. Crozzle is not valid with Test2.cfg. Errors will be logged for each invalid section of data.
 Parse success will be logged.
 Crozzle will display with vlid data displayed and the invalid Crozzle score displayed.</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test3.cfg, Test3.seq, Test3.czl
+    <t>File: Test3.cfg, Test3.seq, Test3.czl
 Data: Appendix G, Appendix H, Appendix I</t>
   </si>
   <si>
-    <t xml:space="preserve">Files will fail to parse due to invalid data.
+    <t>Files will fail to parse due to invalid data.
 Files will not validate successfully. Crozzle is not valid due to invalid data, illegal data, missing data, Test3.cfg invalid. Errors will be logged for every section of invalid and illegal data encountered.
 Crozzle will display with as much valid data as can be found.
 Invalid Crozzle score will be displayed.</t>
   </si>
   <si>
-    <t xml:space="preserve">Crozzle.ToStringHTML()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test1.cfg, Test1.czl
+    <t>Crozzle.ToStringHTML()</t>
+  </si>
+  <si>
+    <t>File: Test1.cfg, Test1.czl
 Data: Appendix A, Appendix C</t>
   </si>
   <si>
-    <t xml:space="preserve">File will parse correctly, all data is valid.
+    <t>File will parse correctly, all data is valid.
 Crozzle.ToStringHTML() will create legal HTML.
 Crozle will display in the given style.</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test2.cfg, Test2.czl
+    <t>File: Test2.cfg, Test2.czl
 Data: Appendix D, Appendix F</t>
   </si>
   <si>
-    <t xml:space="preserve">File will parse correctly, invalid data including duplicate will not be processed. 
+    <t>File will parse correctly, invalid data including duplicate will not be processed. 
 Valid data will be output to HTML string by Crozzle.ToStringHTML() and invalid data will be displayed in error log.</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test3.cfg, Test3.czl
+    <t>File: Test3.cfg, Test3.czl
 Data: Appendix G, Appendix I</t>
   </si>
   <si>
@@ -948,38 +922,38 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">CrozzleMap.GroupCount()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test1.czl
+    <t>CrozzleMap.GroupCount()</t>
+  </si>
+  <si>
+    <t>File: Test1.czl
 Data: Appendix C</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test2.czl
+    <t>File: Test2.czl
 Data: Appendix F</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test3.czl
+    <t>File: Test3.czl
 Data: Appendix I</t>
   </si>
   <si>
-    <t xml:space="preserve">Configuration.TryParse()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test1.cfg
+    <t>Configuration.TryParse()</t>
+  </si>
+  <si>
+    <t>File: Test1.cfg
 Data: Appendix A</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test2.cfg
+    <t>File: Test2.cfg
 Data: Appendix D</t>
   </si>
   <si>
-    <t xml:space="preserve">File will parse correctly.
+    <t>File will parse correctly.
 Contains only logically invalid data.
 Parse success will be logged.</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test3.cfg
+    <t>File: Test3.cfg
 Data: Appendix G</t>
   </si>
   <si>
@@ -997,14 +971,14 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">x</t>
+      <t>x</t>
     </r>
     <r>
       <rPr>
@@ -1014,27 +988,27 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">.” error will be displayed.</t>
+      <t>.” error will be displayed.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">WordList.TryParse()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File: Test1.seq
+    <t>WordList.TryParse()</t>
+  </si>
+  <si>
+    <t>File: Test1.seq
 Data: Appendix B</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test2.seq
+    <t>File: Test2.seq
 Data: Appendix E</t>
   </si>
   <si>
-    <t xml:space="preserve">File will parse correctly. 
+    <t>File will parse correctly. 
 Contains error, sequence JOHNATHON has incorrect ASCII value in ASCII value column. 
 Data technically correct as values add correctly.</t>
   </si>
   <si>
-    <t xml:space="preserve">File: Test3.seq
+    <t>File: Test3.seq
 Data: Appendix H</t>
   </si>
   <si>
@@ -1052,14 +1026,14 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">x</t>
+      <t>x</t>
     </r>
     <r>
       <rPr>
@@ -1069,21 +1043,61 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">.” error will be displayed.</t>
+      <t>.” error will be displayed.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Crozzle.TryParse()</t>
+    <t>Crozzle.TryParse()</t>
+  </si>
+  <si>
+    <t>File will parse correctly and return a GroupCout() of 1.</t>
+  </si>
+  <si>
+    <t>File will parse correctly.
+Invalid data will be displayed in the error log while valid data is processed.
+GroupCount() will return 1 group.</t>
+  </si>
+  <si>
+    <t>File will fail parsing.
+Invalid data will be outpu in the error log.
+GroupCount() will attempt to calculate from the valid data processed.</t>
+  </si>
+  <si>
+    <t>Test3.cfg will log an error when validating this option as there is no valid boolean option present.
+Validator.IsBoolean() will return false.
+Test3.cfg contains invalid data error message will be thrown.
+Crozzle GUI will output all valid sequences in uppercase as default.</t>
+  </si>
+  <si>
+    <t>File: Test2.czl
+Data:
+CROZZLE-SIZE
+    SIZE=1,15
+END-CROZZLE-SIZE</t>
+  </si>
+  <si>
+    <t>Test2.czl will parse as correclty with "1" being a valid size value.
+Validator.IsInt32() will return true as the number is technically a valid Int32.
+Crozzle will log an error for Test2.czl file CROZZLE-SIZE.
+Test2.czl error message will be thrown for an invalid size.</t>
+  </si>
+  <si>
+    <t>Test3.czl will fail parsing and validation.
+Validator.IsInt32() will return false.
+A log message of failing to parse Test3.czl will be added.</t>
+  </si>
+  <si>
+    <t>Test3.cfg will log an error when validating this option as there is no valid hex colour code present.
+Validator.IsHexColourCode() will return false.
+Test3.cfg contains invalid data error message will be thrown.
+Crozzle GUI will output all valid sequences with empty TD element colour #777777 (grey) as default.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1092,22 +1106,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1124,7 +1123,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1132,113 +1131,382 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G36" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:G36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G36" totalsRowShown="0">
+  <autoFilter ref="A1:G36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="S/N"/>
-    <tableColumn id="2" name="Assessment Item"/>
-    <tableColumn id="3" name="Function"/>
-    <tableColumn id="4" name="Input Data"/>
-    <tableColumn id="5" name="Expected Result"/>
-    <tableColumn id="6" name="Actual Output"/>
-    <tableColumn id="7" name="Pass/Fail"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="S/N"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Assessment Item"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Function"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Input Data"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected Result"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Actual Output"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Pass/Fail"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="47.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="39.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="47.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.53"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="47.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
+    <col min="8" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1261,12 +1529,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
-        <f aca="false">TEXT(ROW(A2)-1,"00")</f>
+        <f t="shared" ref="A2:A36" si="0">TEXT(ROW(A2)-1,"00")</f>
         <v>01</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -1281,12 +1549,12 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
-        <f aca="false">TEXT(ROW(A3)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>02</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1296,675 +1564,675 @@
         <v>10</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="str">
-        <f aca="false">TEXT(ROW(A4)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>03</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="6">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
-        <f aca="false">TEXT(ROW(A5)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>04</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="6">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
-        <f aca="false">TEXT(ROW(A6)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>05</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f aca="false">TEXT(ROW(A7)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>06</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="6">
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
-        <f aca="false">TEXT(ROW(A8)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>07</v>
       </c>
-      <c r="B8" s="6" t="n">
+      <c r="B8" s="6">
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
-        <f aca="false">TEXT(ROW(A9)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>08</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="6">
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="406.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
-        <f aca="false">TEXT(ROW(A10)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>09</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="6">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="420" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
-        <f aca="false">TEXT(ROW(A11)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="n">
+      <c r="B11" s="6">
         <v>4</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="406.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
-        <f aca="false">TEXT(ROW(A12)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="n">
+      <c r="B12" s="6">
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="E12" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="200.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:7" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
-        <f aca="false">TEXT(ROW(A13)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="n">
+      <c r="B13" s="6">
         <v>5</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="200.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:7" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
-        <f aca="false">TEXT(ROW(A14)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="n">
+      <c r="B14" s="6">
         <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
-        <f aca="false">TEXT(ROW(A15)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="n">
+      <c r="B15" s="6">
         <v>5</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="200.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:7" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
-        <f aca="false">TEXT(ROW(A16)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="n">
+      <c r="B16" s="6">
         <v>6</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
-        <f aca="false">TEXT(ROW(A17)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="n">
+      <c r="B17" s="6">
         <v>6</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="str">
-        <f aca="false">TEXT(ROW(A18)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="n">
+      <c r="B18" s="6">
         <v>6</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="E18" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="str">
-        <f aca="false">TEXT(ROW(A19)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="n">
+      <c r="B19" s="6">
         <v>7</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="str">
-        <f aca="false">TEXT(ROW(A20)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="n">
+      <c r="B20" s="6">
         <v>7</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="str">
-        <f aca="false">TEXT(ROW(A21)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="n">
+      <c r="B21" s="6">
         <v>7</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="E21" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="str">
-        <f aca="false">TEXT(ROW(A22)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="n">
+      <c r="B22" s="6">
         <v>8</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="str">
-        <f aca="false">TEXT(ROW(A23)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="6" t="n">
+      <c r="B23" s="6">
         <v>8</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="str">
-        <f aca="false">TEXT(ROW(A24)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="6" t="n">
+      <c r="B24" s="6">
         <v>8</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="str">
-        <f aca="false">TEXT(ROW(A25)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="6" t="n">
+      <c r="B25" s="6">
         <v>9</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="str">
-        <f aca="false">TEXT(ROW(A26)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="n">
+      <c r="B26" s="6">
         <v>9</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="str">
-        <f aca="false">TEXT(ROW(A27)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="6" t="n">
+      <c r="B27" s="6">
         <v>9</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="str">
-        <f aca="false">TEXT(ROW(A28)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="6" t="n">
+      <c r="B28" s="6">
         <v>10</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="str">
-        <f aca="false">TEXT(ROW(A29)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="6" t="n">
+      <c r="B29" s="6">
         <v>10</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="str">
-        <f aca="false">TEXT(ROW(A30)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="n">
+      <c r="B30" s="6">
         <v>10</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="str">
-        <f aca="false">TEXT(ROW(A31)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="6" t="n">
+      <c r="B31" s="6">
         <v>11</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="str">
-        <f aca="false">TEXT(ROW(A32)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="6" t="n">
+      <c r="B32" s="6">
         <v>11</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="str">
-        <f aca="false">TEXT(ROW(A33)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="n">
+      <c r="B33" s="6">
         <v>11</v>
       </c>
       <c r="C33" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="str">
-        <f aca="false">TEXT(ROW(A34)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" s="6" t="n">
+      <c r="B34" s="6">
         <v>12</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="str">
-        <f aca="false">TEXT(ROW(A35)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B35" s="6" t="n">
+      <c r="B35" s="6">
         <v>12</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="str">
-        <f aca="false">TEXT(ROW(A36)-1,"00")</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B36" s="6" t="n">
+      <c r="B36" s="6">
         <v>12</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <tableParts>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>

</xml_diff>

<commit_message>
[testing] finalized unit test spreadsheet
</commit_message>
<xml_diff>
--- a/Test Files/Unit Tests.xlsx
+++ b/Test Files/Unit Tests.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arran\Projects\SIT323-Assignment-1\Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{764389C5-C26B-429A-B34C-7408F71D3FC2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{74F99F2C-B064-4D82-8CB0-6B363745306D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="179017" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="82">
   <si>
     <t>S/N</t>
   </si>
@@ -162,43 +162,6 @@
   </si>
   <si>
     <t>File will parse correctly, all data is valid.</t>
-  </si>
-  <si>
-    <t>File: Test2.cfg
-Data:
-INTERSECTING-POINTS
-  A=1
-  B=2
-  C=2
-  D=2
-  E=1
-  F=2
-  G=2
-  H=2
-  I=1
-  J=4
-  K=4
-  L=4
-  M=4
-  N=4
-  O=1
-  P=8
-  Q=8
-  R=8
-  S=8
-  T=8
-  U=1
-  V=16
-  W=16
-  X=32
-  Y=32
-  Z=64
-  z=64
-END-INTERSECTING-POINTS</t>
-  </si>
-  <si>
-    <t>File will parse correctly, contains invalid data with lowercase keyvalue that doesn’t match regular expression.
-KeyValue.TryParse() will return error for this KeyValue.</t>
   </si>
   <si>
     <t>File: Test3.cfg
@@ -650,12 +613,6 @@
 WENDY,10,5,391,406</t>
   </si>
   <si>
-    <t>All files will fail parsing and validation.
-Crozzle.Score() will throw an invalid exception and not return a score.
-An invalid data error will be logged for all test files.
-An error message will be displayed for each error including Test3.cfg invalid intersecting points, Test3.cfg invalid sequence limit, minimum exceeds maximum, Test3.seq invalid data, Test3.czl invalid location.</t>
-  </si>
-  <si>
     <t>CrozzleSequences.CheckDuplicateWords()</t>
   </si>
   <si>
@@ -853,12 +810,6 @@
 WENDY,10,5,391,406</t>
   </si>
   <si>
-    <t>Files will fail to parse with incorrect data, file Test3.czl is invalid due to invalid and data missing.
-CrozzleSequences.CheckDuplicateWords() will return 1 duplicate word.
-Log error for invalid Crozzle due to excessive duplicate words.
-Display error message for duplicate words in Test3.czl word AL with 1 duplicate.</t>
-  </si>
-  <si>
     <t>Crozzle.Validate()</t>
   </si>
   <si>
@@ -876,20 +827,8 @@
 Data: Appendix D, Appendix E, Appendix F</t>
   </si>
   <si>
-    <t>Files will parse correctly.
-Files will not validate successfully. Crozzle is not valid with Test2.cfg. Errors will be logged for each invalid section of data.
-Parse success will be logged.
-Crozzle will display with vlid data displayed and the invalid Crozzle score displayed.</t>
-  </si>
-  <si>
     <t>File: Test3.cfg, Test3.seq, Test3.czl
 Data: Appendix G, Appendix H, Appendix I</t>
-  </si>
-  <si>
-    <t>Files will fail to parse due to invalid data.
-Files will not validate successfully. Crozzle is not valid due to invalid data, illegal data, missing data, Test3.cfg invalid. Errors will be logged for every section of invalid and illegal data encountered.
-Crozzle will display with as much valid data as can be found.
-Invalid Crozzle score will be displayed.</t>
   </si>
   <si>
     <t>Crozzle.ToStringHTML()</t>
@@ -948,48 +887,8 @@
 Data: Appendix D</t>
   </si>
   <si>
-    <t>File will parse correctly.
-Contains only logically invalid data.
-Parse success will be logged.</t>
-  </si>
-  <si>
     <t>File: Test3.cfg
 Data: Appendix G</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">File will fail to parse, contains invalid data.
-Fail to parse will be logged.
-“Error in Test3.cfg at line </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.” error will be displayed.</t>
-    </r>
   </si>
   <si>
     <t>WordList.TryParse()</t>
@@ -1012,45 +911,7 @@
 Data: Appendix H</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">File will fail to parse, contains invalid data.
-Fail to parse will be logged.
-“Error in Test3.czl at line </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.” error will be displayed.</t>
-    </r>
-  </si>
-  <si>
     <t>Crozzle.TryParse()</t>
-  </si>
-  <si>
-    <t>File will parse correctly and return a GroupCout() of 1.</t>
   </si>
   <si>
     <t>File will parse correctly.
@@ -1089,8 +950,95 @@
   <si>
     <t>Test3.cfg will log an error when validating this option as there is no valid hex colour code present.
 Validator.IsHexColourCode() will return false.
-Test3.cfg contains invalid data error message will be thrown.
-Crozzle GUI will output all valid sequences with empty TD element colour #777777 (grey) as default.</t>
+Test3.cfg contains invalid data error message will be thrown.</t>
+  </si>
+  <si>
+    <t>File: Test2.cfg
+Data:
+INTERSECTING-POINTS
+  A=1
+  B=2
+  C=2
+  D=2
+  E=1
+  F=2
+  G=2
+  H=2
+  I=1
+  J=4
+  K=4
+  L=4
+  M=4
+  N=4
+  O=1
+  P=8
+  Q=8
+  R=8
+  S=8
+  T=8
+  U=1
+  V=16
+  W=16
+  X=32
+  Y=32
+  Z=64
+  Z=54
+END-INTERSECTING-POINTS</t>
+  </si>
+  <si>
+    <t>File will parse correctly.
+Contains invalid data with duplicate KeyValue.
+KeyValue.TryParse() will parse this value correctly.</t>
+  </si>
+  <si>
+    <t>All files will fail parsing and validation.
+Crozzle.Score() will throw an invalid exception and not return a score.
+An invalid data error will be logged for all test files.</t>
+  </si>
+  <si>
+    <t>Files will fail to parse with incorrect data, file Test3.czl is invalid due to illegal and missing data.
+CrozzleSequences.CheckDuplicateWords() will return 1 duplicate word.
+Log error for invalid Crozzle due to excessive duplicate words.
+Display error message for duplicate words in Test3.czl word AL with 1 duplicate.</t>
+  </si>
+  <si>
+    <t>Files will parse correctly.
+Files will not validate successfully. Crozzle is not valid with Test2.cfg. Errors will be logged for each invalid section of data.
+Parse success will be logged.
+Crozzle will display with valid data displayed and the invalid Crozzle score displayed.</t>
+  </si>
+  <si>
+    <t>Files will fail to parse due to invalid data.
+Files will not validate successfully. 
+Crozzle is not valid due to invalid data, illegal data, missing data, Test3.cfg invalid. 
+Errors will be logged for every section of invalid and illegal data encountered.
+Crozzle will display with as much valid data as can be found.
+Invalid Crozzle score will be displayed.</t>
+  </si>
+  <si>
+    <t>File will parse correctly and return a GroupCount() of 1.</t>
+  </si>
+  <si>
+    <t>File will parse correctly.
+Contains only logically invalid data.
+Parse success will be logged.
+Invalid data will be logged.</t>
+  </si>
+  <si>
+    <t>File will fail to parse, contains illegal data.
+Fail to parse will be logged.
+Error will be displayed for all invalid data entries</t>
+  </si>
+  <si>
+    <t>File will fail to parse, contains illegal data.
+Fail to parse will be logged.
+Error will be displayed for all illegal data entries.</t>
+  </si>
+  <si>
+    <t>File will parse correctly.
+Contains only logically invalid data.
+Parse success will be logged.
+Error will be displayed for all illegal data entries</t>
   </si>
 </sst>
 </file>
@@ -1489,9 +1437,9 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1512,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -1601,10 +1549,10 @@
         <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -1624,7 +1572,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1669,7 +1617,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f t="shared" si="0"/>
         <v>08</v>
@@ -1684,7 +1632,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -1721,10 +1669,10 @@
         <v>21</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -1741,10 +1689,10 @@
         <v>21</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -1758,13 +1706,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -1778,13 +1726,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -1798,13 +1746,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1818,13 +1766,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -1838,13 +1786,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="E17" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1858,13 +1806,13 @@
         <v>6</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1878,13 +1826,13 @@
         <v>7</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1898,18 +1846,18 @@
         <v>7</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="str">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1918,13 +1866,13 @@
         <v>7</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="E21" s="5" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -1938,13 +1886,13 @@
         <v>8</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -1958,13 +1906,13 @@
         <v>8</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -1978,13 +1926,13 @@
         <v>8</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1998,13 +1946,13 @@
         <v>9</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -2018,13 +1966,13 @@
         <v>9</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -2038,13 +1986,13 @@
         <v>9</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -2058,10 +2006,10 @@
         <v>10</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>23</v>
@@ -2069,7 +2017,7 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="str">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2078,18 +2026,18 @@
         <v>10</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="str">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2098,13 +2046,13 @@
         <v>10</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -2118,10 +2066,10 @@
         <v>11</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>23</v>
@@ -2138,13 +2086,13 @@
         <v>11</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -2158,13 +2106,13 @@
         <v>11</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -2178,10 +2126,10 @@
         <v>12</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>23</v>
@@ -2189,7 +2137,7 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="str">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2198,13 +2146,13 @@
         <v>12</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -2218,13 +2166,13 @@
         <v>12</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>

</xml_diff>